<commit_message>
AI architecture dead end
</commit_message>
<xml_diff>
--- a/IAUS Architecture.xlsx
+++ b/IAUS Architecture.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unity\Vermetio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{103A0392-1EF6-4632-96CE-E901CF2BC33E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630617A4-E7A4-4201-BEF3-C3C4A7EFB8AC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="27">
   <si>
     <t>CurveType</t>
   </si>
@@ -100,26 +100,29 @@
     <t>IActionIComponents</t>
   </si>
   <si>
-    <t>component per action
-can't be buffer or array?</t>
-  </si>
-  <si>
     <t>IActionIComponent has blob ref to ActionDef</t>
   </si>
   <si>
     <t>ActionDef[]</t>
   </si>
   <si>
-    <t>based on score add currect Action tag</t>
-  </si>
-  <si>
     <t>Inifite Axis Utility System</t>
+  </si>
+  <si>
+    <t>component per action</t>
+  </si>
+  <si>
+    <t>CurrentAction:
+    BlobRef (maybe add int Id instead)</t>
+  </si>
+  <si>
+    <t>Generic action scoring job?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -137,7 +140,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,6 +150,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -178,18 +187,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -205,6 +208,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -518,11 +528,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +548,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>13</v>
@@ -548,20 +558,23 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="H2" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="2"/>
@@ -579,13 +592,13 @@
       <c r="E6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="10" t="s">
         <v>6</v>
       </c>
     </row>
@@ -595,10 +608,10 @@
       <c r="E7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="3"/>
+      <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
@@ -606,13 +619,13 @@
       <c r="E8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="3"/>
+      <c r="H8" s="11"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H9" t="s">
+      <c r="H9" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -621,9 +634,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
-        <v>21</v>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
@@ -631,27 +644,27 @@
       <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>24</v>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C13" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -661,7 +674,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Megablob of all actions, probably bad idea, was supposed to work around blob corruption in job
</commit_message>
<xml_diff>
--- a/IAUS Architecture.xlsx
+++ b/IAUS Architecture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unity\Vermetio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630617A4-E7A4-4201-BEF3-C3C4A7EFB8AC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90248A8F-CDB8-4E0D-BFDE-89E2D266257B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>CurveType</t>
   </si>
@@ -204,17 +204,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -532,7 +532,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +558,7 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -625,7 +625,7 @@
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -635,7 +635,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C11" t="s">
@@ -644,7 +644,7 @@
       <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F11" s="3" t="s">

</xml_diff>